<commit_message>
Detection probability raster maps for all years
</commit_message>
<xml_diff>
--- a/technicalReports/fagrapport104_Detection2025/output/tables/OverallDetectability.xlsx
+++ b/technicalReports/fagrapport104_Detection2025/output/tables/OverallDetectability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduumb-my.sharepoint.com/personal/asuncion_semper_pascual_nmbu_no/Documents/02_RovQuant/03_Reports/DetectionProbability/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seasunci\03_RovQuant_Public\RovQuantPublic\technicalReports\fagrapport104_Detection2025\output\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51108EE7-052A-45DC-A77D-6536BC96C1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40D6064-759D-418C-91FA-13C604A406CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29EE2423-DC44-430F-9C92-CCF7E25F1CDB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{29EE2423-DC44-430F-9C92-CCF7E25F1CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
-  <si>
-    <t xml:space="preserve"> 0.70 (0.63-0.77)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t xml:space="preserve"> 0.60 (0.53-0.67)</t>
   </si>
@@ -74,9 +71,6 @@
     <t>WOLF</t>
   </si>
   <si>
-    <t xml:space="preserve">0.49 (0.45-0.54) </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.53 (0.49-0.57) </t>
   </si>
   <si>
@@ -125,16 +119,10 @@
     <t xml:space="preserve"> 2023/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">2014/2015 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2015/2016 </t>
   </si>
   <si>
     <t xml:space="preserve"> 2016/2017 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.50 (0.46-0.55) </t>
   </si>
   <si>
     <t xml:space="preserve"> 0.75 (0.71-0.79) </t>
@@ -214,13 +202,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,56 +544,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B777FE-9677-474C-9D45-6B0991FAB259}">
-  <dimension ref="A2:K7"/>
+  <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C2" s="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
         <v>2015</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C2" s="1">
         <v>2016</v>
       </c>
-      <c r="E2" s="2">
+      <c r="D2" s="1">
         <v>2017</v>
       </c>
-      <c r="F2" s="2">
+      <c r="E2" s="1">
         <v>2018</v>
       </c>
-      <c r="G2" s="2">
+      <c r="F2" s="1">
         <v>2019</v>
       </c>
-      <c r="H2" s="2">
+      <c r="G2" s="1">
         <v>2020</v>
       </c>
-      <c r="I2" s="2">
+      <c r="H2" s="1">
         <v>2021</v>
       </c>
-      <c r="J2" s="2">
+      <c r="I2" s="1">
         <v>2022</v>
       </c>
-      <c r="K2" s="2">
+      <c r="J2" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -613,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -633,144 +617,129 @@
       <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2022</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2023</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2016</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2017</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2018</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2019</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2020</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2021</v>
-      </c>
-      <c r="I4" s="3">
-        <v>2022</v>
-      </c>
-      <c r="J4" s="3">
-        <v>2023</v>
-      </c>
-      <c r="K4" s="3">
-        <v>2024</v>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>